<commit_message>
final update moving on to another project
</commit_message>
<xml_diff>
--- a/src/Grouptime.xlsx
+++ b/src/Grouptime.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ad687a3ac9ee377/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ad687a3ac9ee377/Desktop/Group Time React app/group-time/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_178DD4AC4547ADF6B36A8BAC57F4724754CD2033" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5CF5E36-BB10-4C86-90F7-E738F082DDE4}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_178DD4AC4547ADF6B36A8BAC57F4724754CD2033" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD0B0336-EA70-4F41-A30E-5FCB05131C99}"/>
   <bookViews>
-    <workbookView xWindow="-25080" yWindow="1260" windowWidth="23910" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27945" yWindow="840" windowWidth="27240" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Group 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Group 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -598,7 +600,7 @@
   <dimension ref="A1:M111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1176,4 +1178,30 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663816E9-C27C-4780-BD72-440173117373}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1343E7-B77B-4EEB-B8AA-FF7B1B193C9B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>